<commit_message>
Updated units and database
- Updated the calculations for GDP and Energy Intensity to receive results in mio €
- Updated database for different EPG gaps
- Resolved reuse compliane issue with missing licence in obsolete and redundant .csv file
</commit_message>
<xml_diff>
--- a/src/micat/template/measure_specific_parameters_template.xlsx
+++ b/src/micat/template/measure_specific_parameters_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ren\Documents\_!Projekte\_SEEDMICAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\src\micat\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87DDE55-1F0C-402C-B0EB-C3DC42243A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F17407C-0BB4-4BC1-B71C-277DA284377A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50190" yWindow="0" windowWidth="34185" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="43200" windowHeight="11235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Average rent of energy poor households</t>
-  </si>
-  <si>
-    <t>€</t>
   </si>
   <si>
     <t>% of rent</t>
@@ -244,6 +241,9 @@
   <si>
     <t>id_sector</t>
   </si>
+  <si>
+    <t>€/year</t>
+  </si>
 </sst>
 </file>
 
@@ -326,8 +326,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="60 % - Akzent3" xfId="1" builtinId="40"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -611,23 +611,23 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -636,10 +636,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1">
         <v>2020</v>
@@ -657,7 +657,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3" t="s">
@@ -667,7 +667,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="3">
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>40</v>
       </c>
@@ -695,10 +695,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="3" t="e">
@@ -722,19 +722,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>35</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="3" t="e">
@@ -758,19 +758,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>36</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" t="e">
         <f>NA()</f>
@@ -782,7 +782,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>16</v>
       </c>
@@ -790,13 +790,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="3" t="e">
@@ -820,7 +820,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>16</v>
       </c>
@@ -828,13 +828,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="3" t="e">
@@ -858,7 +858,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>16</v>
       </c>
@@ -866,13 +866,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="3" t="e">
@@ -896,7 +896,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>16</v>
       </c>
@@ -904,13 +904,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="3" t="e">
@@ -934,7 +934,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>16</v>
       </c>
@@ -942,13 +942,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="3" t="e">
@@ -972,7 +972,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>16</v>
       </c>
@@ -980,13 +980,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="3" t="e">
@@ -1010,7 +1010,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>16</v>
       </c>
@@ -1018,13 +1018,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="3" t="e">
@@ -1062,27 +1062,27 @@
       <selection activeCell="Q129" sqref="Q129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1091,7 +1091,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1">
         <v>2010</v>
@@ -1115,7 +1115,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>17</v>
       </c>
@@ -1126,13 +1126,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
@@ -1156,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>17</v>
       </c>
@@ -1167,13 +1167,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>17</v>
       </c>
@@ -1208,13 +1208,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -1238,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>17</v>
       </c>
@@ -1249,13 +1249,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>100</v>
@@ -1279,7 +1279,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>17</v>
       </c>
@@ -1290,54 +1290,54 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -1361,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>17</v>
       </c>
@@ -1372,13 +1372,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1402,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>18</v>
       </c>
@@ -1413,13 +1413,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -1443,7 +1443,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>18</v>
       </c>
@@ -1454,13 +1454,13 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>18</v>
       </c>
@@ -1495,13 +1495,13 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>18</v>
       </c>
@@ -1536,13 +1536,13 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1566,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>18</v>
       </c>
@@ -1577,13 +1577,13 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1607,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>18</v>
       </c>
@@ -1618,13 +1618,13 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1648,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>18</v>
       </c>
@@ -1659,13 +1659,13 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1700,13 +1700,13 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" s="3">
         <v>1</v>
@@ -1730,7 +1730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1741,13 +1741,13 @@
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" s="3">
         <v>0.9</v>
@@ -1771,7 +1771,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -1782,13 +1782,13 @@
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" s="3">
         <v>0.88</v>
@@ -1812,7 +1812,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -1823,13 +1823,13 @@
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" s="3">
         <v>0.9</v>
@@ -1853,7 +1853,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>14</v>
       </c>
@@ -1864,13 +1864,13 @@
         <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" s="3">
         <v>0.88</v>
@@ -1894,7 +1894,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>14</v>
       </c>
@@ -1905,13 +1905,13 @@
         <v>6</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" s="3">
         <v>0.9</v>
@@ -1935,7 +1935,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -1946,13 +1946,13 @@
         <v>7</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" s="3">
         <v>0.9</v>
@@ -1976,7 +1976,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
@@ -1987,13 +1987,13 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23">
         <v>1.5</v>
@@ -2017,7 +2017,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -2028,13 +2028,13 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24">
         <v>0.94</v>
@@ -2058,7 +2058,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>15</v>
       </c>
@@ -2069,13 +2069,13 @@
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G25">
         <v>0.9</v>
@@ -2099,7 +2099,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>15</v>
       </c>
@@ -2110,13 +2110,13 @@
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G26">
         <v>0.93</v>
@@ -2140,7 +2140,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15</v>
       </c>
@@ -2151,13 +2151,13 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27">
         <v>0.9</v>
@@ -2181,7 +2181,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>15</v>
       </c>
@@ -2192,13 +2192,13 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G28">
         <v>0.92</v>
@@ -2222,7 +2222,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
@@ -2233,13 +2233,13 @@
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G29">
         <v>0.93</v>
@@ -2263,7 +2263,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>17</v>
       </c>
@@ -2274,13 +2274,13 @@
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G30" s="3">
         <v>0</v>
@@ -2304,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>17</v>
       </c>
@@ -2315,13 +2315,13 @@
         <v>2</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -2356,13 +2356,13 @@
         <v>3</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G32" s="3">
         <v>0</v>
@@ -2386,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>17</v>
       </c>
@@ -2397,13 +2397,13 @@
         <v>4</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G33" s="3">
         <v>100</v>
@@ -2427,7 +2427,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>17</v>
       </c>
@@ -2438,13 +2438,13 @@
         <v>5</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G34" s="3">
         <v>0</v>
@@ -2468,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
@@ -2479,13 +2479,13 @@
         <v>6</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
@@ -2509,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>17</v>
       </c>
@@ -2520,13 +2520,13 @@
         <v>7</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G36" s="3">
         <v>0</v>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>18</v>
       </c>
@@ -2561,13 +2561,13 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G37">
         <v>100</v>
@@ -2591,7 +2591,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>18</v>
       </c>
@@ -2602,13 +2602,13 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2632,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>18</v>
       </c>
@@ -2643,13 +2643,13 @@
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2673,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>18</v>
       </c>
@@ -2684,13 +2684,13 @@
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>18</v>
       </c>
@@ -2725,13 +2725,13 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2755,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>18</v>
       </c>
@@ -2766,13 +2766,13 @@
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -2796,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>18</v>
       </c>
@@ -2807,13 +2807,13 @@
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -2837,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>14</v>
       </c>
@@ -2848,13 +2848,13 @@
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G44" s="3">
         <v>1</v>
@@ -2878,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>14</v>
       </c>
@@ -2889,13 +2889,13 @@
         <v>2</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G45" s="3">
         <v>0.9</v>
@@ -2919,7 +2919,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>14</v>
       </c>
@@ -2930,13 +2930,13 @@
         <v>3</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G46" s="3">
         <v>0.88</v>
@@ -2960,7 +2960,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>14</v>
       </c>
@@ -2971,13 +2971,13 @@
         <v>4</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G47" s="3">
         <v>0.9</v>
@@ -3001,7 +3001,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>14</v>
       </c>
@@ -3012,13 +3012,13 @@
         <v>5</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G48" s="3">
         <v>0.88</v>
@@ -3042,7 +3042,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>14</v>
       </c>
@@ -3053,13 +3053,13 @@
         <v>6</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G49" s="3">
         <v>0.9</v>
@@ -3083,7 +3083,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>14</v>
       </c>
@@ -3094,13 +3094,13 @@
         <v>7</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G50" s="3">
         <v>0.9</v>
@@ -3124,7 +3124,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -3135,13 +3135,13 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G51">
         <v>1.5</v>
@@ -3165,7 +3165,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>15</v>
       </c>
@@ -3176,13 +3176,13 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G52">
         <v>0.94</v>
@@ -3206,7 +3206,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>15</v>
       </c>
@@ -3217,13 +3217,13 @@
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G53">
         <v>0.9</v>
@@ -3247,7 +3247,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>15</v>
       </c>
@@ -3258,13 +3258,13 @@
         <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G54">
         <v>0.93</v>
@@ -3288,7 +3288,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>15</v>
       </c>
@@ -3299,13 +3299,13 @@
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G55">
         <v>0.9</v>
@@ -3329,7 +3329,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>15</v>
       </c>
@@ -3340,13 +3340,13 @@
         <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G56">
         <v>0.92</v>
@@ -3370,7 +3370,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>15</v>
       </c>
@@ -3381,13 +3381,13 @@
         <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G57">
         <v>0.93</v>
@@ -3411,7 +3411,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>17</v>
       </c>
@@ -3422,13 +3422,13 @@
         <v>1</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G58" s="3">
         <v>0</v>
@@ -3452,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>17</v>
       </c>
@@ -3463,13 +3463,13 @@
         <v>2</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G59" s="3">
         <v>30</v>
@@ -3493,7 +3493,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>17</v>
       </c>
@@ -3504,13 +3504,13 @@
         <v>3</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G60" s="3">
         <v>10</v>
@@ -3534,7 +3534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>17</v>
       </c>
@@ -3545,13 +3545,13 @@
         <v>4</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G61" s="3">
         <v>60</v>
@@ -3575,7 +3575,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>17</v>
       </c>
@@ -3586,13 +3586,13 @@
         <v>5</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G62" s="3">
         <v>0</v>
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>17</v>
       </c>
@@ -3627,13 +3627,13 @@
         <v>6</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G63" s="3">
         <v>0</v>
@@ -3657,7 +3657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>17</v>
       </c>
@@ -3668,13 +3668,13 @@
         <v>7</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G64" s="3">
         <v>0</v>
@@ -3698,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>18</v>
       </c>
@@ -3709,13 +3709,13 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G65">
         <v>100</v>
@@ -3739,7 +3739,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>18</v>
       </c>
@@ -3750,13 +3750,13 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -3780,7 +3780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>18</v>
       </c>
@@ -3791,13 +3791,13 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>18</v>
       </c>
@@ -3832,13 +3832,13 @@
         <v>4</v>
       </c>
       <c r="D68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -3862,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>18</v>
       </c>
@@ -3873,13 +3873,13 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -3903,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>18</v>
       </c>
@@ -3914,13 +3914,13 @@
         <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -3944,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>18</v>
       </c>
@@ -3955,13 +3955,13 @@
         <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3985,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>14</v>
       </c>
@@ -3996,13 +3996,13 @@
         <v>1</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G72" s="3">
         <v>1</v>
@@ -4026,7 +4026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>14</v>
       </c>
@@ -4037,13 +4037,13 @@
         <v>2</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G73" s="3">
         <v>0.86449999999999994</v>
@@ -4067,7 +4067,7 @@
         <v>0.90249999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>14</v>
       </c>
@@ -4078,13 +4078,13 @@
         <v>3</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G74" s="3">
         <v>0.42749999999999999</v>
@@ -4108,7 +4108,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>14</v>
       </c>
@@ -4119,13 +4119,13 @@
         <v>4</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G75" s="3">
         <v>0.93099999999999994</v>
@@ -4149,7 +4149,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>14</v>
       </c>
@@ -4160,13 +4160,13 @@
         <v>5</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G76" s="3">
         <v>0.7932499999999999</v>
@@ -4190,7 +4190,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>14</v>
       </c>
@@ -4201,13 +4201,13 @@
         <v>6</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G77" s="3">
         <v>0.93669999999999998</v>
@@ -4231,7 +4231,7 @@
         <v>0.94524999999999992</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>14</v>
       </c>
@@ -4242,13 +4242,13 @@
         <v>7</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G78" s="3">
         <v>0.93955</v>
@@ -4272,7 +4272,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>15</v>
       </c>
@@ -4283,13 +4283,13 @@
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G79">
         <v>3.0250000000000004</v>
@@ -4313,7 +4313,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>15</v>
       </c>
@@ -4324,13 +4324,13 @@
         <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G80">
         <v>0.91</v>
@@ -4354,7 +4354,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>15</v>
       </c>
@@ -4365,13 +4365,13 @@
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G81">
         <v>0.45</v>
@@ -4395,7 +4395,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>15</v>
       </c>
@@ -4406,13 +4406,13 @@
         <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G82">
         <v>0.98</v>
@@ -4436,7 +4436,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>15</v>
       </c>
@@ -4447,13 +4447,13 @@
         <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G83">
         <v>0.83499999999999996</v>
@@ -4477,7 +4477,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>15</v>
       </c>
@@ -4488,13 +4488,13 @@
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G84">
         <v>0.98599999999999999</v>
@@ -4518,7 +4518,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>15</v>
       </c>
@@ -4529,13 +4529,13 @@
         <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G85">
         <v>0.98899999999999999</v>
@@ -4559,7 +4559,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>17</v>
       </c>
@@ -4570,13 +4570,13 @@
         <v>1</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G86" s="3">
         <v>0</v>
@@ -4600,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>17</v>
       </c>
@@ -4611,13 +4611,13 @@
         <v>2</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G87" s="3">
         <v>30</v>
@@ -4641,7 +4641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>17</v>
       </c>
@@ -4652,13 +4652,13 @@
         <v>3</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G88" s="3">
         <v>10</v>
@@ -4682,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>17</v>
       </c>
@@ -4693,13 +4693,13 @@
         <v>4</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G89" s="3">
         <v>60</v>
@@ -4723,7 +4723,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>17</v>
       </c>
@@ -4734,13 +4734,13 @@
         <v>5</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G90" s="3">
         <v>0</v>
@@ -4764,7 +4764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>17</v>
       </c>
@@ -4775,13 +4775,13 @@
         <v>6</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G91" s="3">
         <v>0</v>
@@ -4805,7 +4805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>17</v>
       </c>
@@ -4816,13 +4816,13 @@
         <v>7</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G92" s="3">
         <v>0</v>
@@ -4846,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>18</v>
       </c>
@@ -4857,13 +4857,13 @@
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F93" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G93">
         <v>100</v>
@@ -4887,7 +4887,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>18</v>
       </c>
@@ -4898,13 +4898,13 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4928,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>18</v>
       </c>
@@ -4939,13 +4939,13 @@
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F95" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -4969,7 +4969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>18</v>
       </c>
@@ -4980,13 +4980,13 @@
         <v>4</v>
       </c>
       <c r="D96" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F96" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -5010,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>18</v>
       </c>
@@ -5021,13 +5021,13 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F97" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -5051,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>18</v>
       </c>
@@ -5062,13 +5062,13 @@
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F98" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -5092,7 +5092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>18</v>
       </c>
@@ -5103,13 +5103,13 @@
         <v>7</v>
       </c>
       <c r="D99" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F99" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -5133,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>14</v>
       </c>
@@ -5144,13 +5144,13 @@
         <v>1</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G100" s="3">
         <v>1</v>
@@ -5174,7 +5174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>14</v>
       </c>
@@ -5185,13 +5185,13 @@
         <v>2</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G101" s="3">
         <v>0.86449999999999994</v>
@@ -5215,7 +5215,7 @@
         <v>0.90249999999999997</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>14</v>
       </c>
@@ -5226,13 +5226,13 @@
         <v>3</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G102" s="3">
         <v>0.42749999999999999</v>
@@ -5256,7 +5256,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>14</v>
       </c>
@@ -5267,13 +5267,13 @@
         <v>4</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G103" s="3">
         <v>0.93099999999999994</v>
@@ -5297,7 +5297,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>14</v>
       </c>
@@ -5308,13 +5308,13 @@
         <v>5</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G104" s="3">
         <v>0.7932499999999999</v>
@@ -5338,7 +5338,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>14</v>
       </c>
@@ -5349,13 +5349,13 @@
         <v>6</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G105" s="3">
         <v>0.93669999999999998</v>
@@ -5379,7 +5379,7 @@
         <v>0.94524999999999992</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>14</v>
       </c>
@@ -5390,13 +5390,13 @@
         <v>7</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G106" s="3">
         <v>0.93955</v>
@@ -5420,7 +5420,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>15</v>
       </c>
@@ -5431,13 +5431,13 @@
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G107">
         <v>3.0250000000000004</v>
@@ -5461,7 +5461,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>15</v>
       </c>
@@ -5472,13 +5472,13 @@
         <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G108">
         <v>0.91</v>
@@ -5502,7 +5502,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>15</v>
       </c>
@@ -5513,13 +5513,13 @@
         <v>3</v>
       </c>
       <c r="D109" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G109">
         <v>0.45</v>
@@ -5543,7 +5543,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>15</v>
       </c>
@@ -5554,13 +5554,13 @@
         <v>4</v>
       </c>
       <c r="D110" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G110">
         <v>0.98</v>
@@ -5584,7 +5584,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>15</v>
       </c>
@@ -5595,13 +5595,13 @@
         <v>5</v>
       </c>
       <c r="D111" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G111">
         <v>0.83499999999999996</v>
@@ -5625,7 +5625,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>15</v>
       </c>
@@ -5636,13 +5636,13 @@
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G112">
         <v>0.98599999999999999</v>
@@ -5666,7 +5666,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>15</v>
       </c>
@@ -5677,13 +5677,13 @@
         <v>7</v>
       </c>
       <c r="D113" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F113" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G113">
         <v>0.98899999999999999</v>
@@ -5707,7 +5707,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>17</v>
       </c>
@@ -5718,13 +5718,13 @@
         <v>1</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G114" s="3">
         <v>0</v>
@@ -5748,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>17</v>
       </c>
@@ -5759,13 +5759,13 @@
         <v>2</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G115" s="3">
         <v>100</v>
@@ -5789,7 +5789,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>17</v>
       </c>
@@ -5800,13 +5800,13 @@
         <v>3</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G116" s="3">
         <v>0</v>
@@ -5830,7 +5830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>17</v>
       </c>
@@ -5841,13 +5841,13 @@
         <v>4</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G117" s="3">
         <v>0</v>
@@ -5871,7 +5871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>17</v>
       </c>
@@ -5882,13 +5882,13 @@
         <v>5</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G118" s="3">
         <v>0</v>
@@ -5912,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>17</v>
       </c>
@@ -5923,13 +5923,13 @@
         <v>6</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G119" s="3">
         <v>0</v>
@@ -5953,7 +5953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>17</v>
       </c>
@@ -5964,13 +5964,13 @@
         <v>7</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G120" s="3">
         <v>0</v>
@@ -5994,7 +5994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>18</v>
       </c>
@@ -6005,13 +6005,13 @@
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F121" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G121">
         <v>100</v>
@@ -6035,7 +6035,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>18</v>
       </c>
@@ -6046,13 +6046,13 @@
         <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F122" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -6076,7 +6076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>18</v>
       </c>
@@ -6087,13 +6087,13 @@
         <v>3</v>
       </c>
       <c r="D123" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F123" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -6117,7 +6117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>18</v>
       </c>
@@ -6128,13 +6128,13 @@
         <v>4</v>
       </c>
       <c r="D124" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F124" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -6158,7 +6158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>18</v>
       </c>
@@ -6169,13 +6169,13 @@
         <v>5</v>
       </c>
       <c r="D125" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F125" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -6199,7 +6199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>18</v>
       </c>
@@ -6210,13 +6210,13 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F126" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -6240,7 +6240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>18</v>
       </c>
@@ -6251,13 +6251,13 @@
         <v>7</v>
       </c>
       <c r="D127" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F127" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G127">
         <v>0</v>
@@ -6281,7 +6281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>14</v>
       </c>
@@ -6292,13 +6292,13 @@
         <v>1</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G128" s="3">
         <v>0.65</v>
@@ -6322,7 +6322,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>14</v>
       </c>
@@ -6333,13 +6333,13 @@
         <v>2</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G129" s="3">
         <v>0.28000000000000003</v>
@@ -6363,7 +6363,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>14</v>
       </c>
@@ -6374,13 +6374,13 @@
         <v>3</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G130" s="3">
         <v>0.14000000000000001</v>
@@ -6409,7 +6409,7 @@
       <c r="R130" s="7"/>
       <c r="S130" s="7"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>14</v>
       </c>
@@ -6420,13 +6420,13 @@
         <v>4</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G131" s="3">
         <v>0.38</v>
@@ -6450,7 +6450,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>14</v>
       </c>
@@ -6461,13 +6461,13 @@
         <v>5</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G132" s="3">
         <v>0.14000000000000001</v>
@@ -6491,7 +6491,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>14</v>
       </c>
@@ -6502,13 +6502,13 @@
         <v>6</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G133" s="3">
         <v>0</v>
@@ -6532,7 +6532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>14</v>
       </c>
@@ -6543,13 +6543,13 @@
         <v>7</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G134" s="3">
         <v>0.38</v>
@@ -6573,7 +6573,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>15</v>
       </c>
@@ -6584,13 +6584,13 @@
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F135" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G135">
         <v>0.75</v>
@@ -6614,7 +6614,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>15</v>
       </c>
@@ -6625,13 +6625,13 @@
         <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F136" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G136">
         <v>0.3</v>
@@ -6655,7 +6655,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>15</v>
       </c>
@@ -6666,13 +6666,13 @@
         <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F137" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G137">
         <v>0.15</v>
@@ -6696,7 +6696,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>15</v>
       </c>
@@ -6707,13 +6707,13 @@
         <v>4</v>
       </c>
       <c r="D138" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F138" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G138">
         <v>0.4</v>
@@ -6737,7 +6737,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>15</v>
       </c>
@@ -6748,13 +6748,13 @@
         <v>5</v>
       </c>
       <c r="D139" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F139" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G139">
         <v>0.15</v>
@@ -6778,7 +6778,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>15</v>
       </c>
@@ -6789,13 +6789,13 @@
         <v>6</v>
       </c>
       <c r="D140" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F140" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G140">
         <v>0</v>
@@ -6819,7 +6819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>15</v>
       </c>
@@ -6830,13 +6830,13 @@
         <v>7</v>
       </c>
       <c r="D141" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F141" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G141">
         <v>0.4</v>
@@ -6871,31 +6871,31 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="2" max="2" width="40.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
-    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" customWidth="1"/>
-    <col min="13" max="13" width="18.453125" customWidth="1"/>
-    <col min="14" max="14" width="16.26953125" customWidth="1"/>
-    <col min="15" max="15" width="17.81640625" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -6904,7 +6904,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1">
         <v>2020</v>
@@ -6922,18 +6922,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="e">
         <f>NA()</f>
@@ -6956,7 +6956,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>42</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="e">
         <f>NA()</f>
@@ -6990,7 +6990,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>32</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3" t="e">
         <f>NA()</f>
@@ -7024,7 +7024,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>43</v>
       </c>
@@ -7035,7 +7035,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="e">
         <f>NA()</f>
@@ -7058,7 +7058,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>31</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3" t="e">
         <f>NA()</f>
@@ -7092,7 +7092,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>29</v>
       </c>
@@ -7100,10 +7100,10 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="e">
         <f>NA()</f>
@@ -7126,18 +7126,18 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="e">
         <f>NA()</f>
@@ -7173,42 +7173,42 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="B3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="B4" s="3" t="e">
         <f>NA()</f>

</xml_diff>

<commit_message>
fix: improved some error notifications
</commit_message>
<xml_diff>
--- a/src/micat/template/measure_specific_parameters_template.xlsx
+++ b/src/micat/template/measure_specific_parameters_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\src\micat\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenz/Projekte/micat/src/micat/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F17407C-0BB4-4BC1-B71C-277DA284377A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F7D4CB-FF52-534F-92D0-2FF087E0A8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="43200" windowHeight="11235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1180" windowWidth="34560" windowHeight="11240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -326,8 +326,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60 % - Akzent3" xfId="1" builtinId="40"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -611,18 +611,18 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
     <col min="7" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -657,7 +657,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3" t="s">
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>40</v>
       </c>
@@ -722,7 +722,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>35</v>
       </c>
@@ -758,7 +758,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>36</v>
       </c>
@@ -782,7 +782,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>16</v>
       </c>
@@ -820,7 +820,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>16</v>
       </c>
@@ -858,7 +858,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>16</v>
       </c>
@@ -896,7 +896,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>16</v>
       </c>
@@ -934,7 +934,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>16</v>
       </c>
@@ -972,7 +972,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>16</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>16</v>
       </c>
@@ -1062,19 +1062,19 @@
       <selection activeCell="Q129" sqref="Q129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>17</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>17</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>17</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>17</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>17</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>17</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>17</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>18</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>18</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>18</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>18</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>18</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>18</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>18</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>14</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>14</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>15</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>15</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>15</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>15</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>15</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>15</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>15</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>17</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>17</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>17</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>17</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>17</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>17</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>18</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>18</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>18</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>18</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>18</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>18</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>18</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>14</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>14</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>14</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>14</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>14</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>14</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>14</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>15</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>15</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>15</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>15</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>15</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>15</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>15</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>17</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>17</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>17</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>17</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>17</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>17</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>17</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>18</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>18</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>18</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>18</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>18</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>18</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>18</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>14</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>14</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>0.90249999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>14</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>14</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>14</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>14</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>0.94524999999999992</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>14</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>15</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>15</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>15</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>15</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>15</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>15</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>15</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>17</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>17</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>17</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>17</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>17</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>17</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>17</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>18</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>18</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>18</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>18</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>18</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>18</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>18</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>14</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>14</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>0.90249999999999997</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>14</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>14</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>14</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>14</v>
       </c>
@@ -5379,7 +5379,7 @@
         <v>0.94524999999999992</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>14</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>15</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>15</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>15</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>15</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>15</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>15</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>15</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>17</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>17</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>17</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>17</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>17</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>17</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>17</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>18</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>18</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>18</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>18</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>18</v>
       </c>
@@ -6199,7 +6199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>18</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>18</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>14</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>14</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>14</v>
       </c>
@@ -6409,7 +6409,7 @@
       <c r="R130" s="7"/>
       <c r="S130" s="7"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>14</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>14</v>
       </c>
@@ -6491,7 +6491,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>14</v>
       </c>
@@ -6532,7 +6532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>14</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>15</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>15</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>15</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>15</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>15</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>15</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>15</v>
       </c>
@@ -6871,29 +6871,29 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="22.5" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="18.5" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>45</v>
       </c>
@@ -6956,109 +6956,109 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>32</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F4" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G4" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H4" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I4" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>43</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>31</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>29</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>34</v>
       </c>
@@ -7173,13 +7173,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
feat: added affected fuel category to advanced parameters
</commit_message>
<xml_diff>
--- a/src/micat/template/measure_specific_parameters_template.xlsx
+++ b/src/micat/template/measure_specific_parameters_template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\src\micat\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenz/Projekte/micat/src/micat/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3653AC9-1503-4557-9F8B-2432872CE93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E7E26B-7F9C-C740-B188-647C07CF3901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
-    <sheet name="fuelSwitch" sheetId="1" r:id="rId2"/>
-    <sheet name="residential" sheetId="3" r:id="rId3"/>
-    <sheet name="context" sheetId="4" r:id="rId4"/>
+    <sheet name="affectedFuels" sheetId="5" r:id="rId2"/>
+    <sheet name="fuelSwitch" sheetId="1" r:id="rId3"/>
+    <sheet name="residential" sheetId="3" r:id="rId4"/>
+    <sheet name="context" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="68">
   <si>
     <t>label</t>
   </si>
@@ -326,8 +327,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60 % - Akzent3" xfId="1" builtinId="40"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -605,24 +606,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="A6" sqref="A6:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
     <col min="7" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -657,7 +658,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3" t="s">
@@ -686,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>40</v>
       </c>
@@ -722,7 +723,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>35</v>
       </c>
@@ -758,7 +759,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>36</v>
       </c>
@@ -781,272 +782,6 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H6" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I6" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J6" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K6" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H7" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I7" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J7" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K7" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H8" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I8" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J8" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K8" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H9" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I9" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J9" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K9" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H10" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I10" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J10" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K10" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H11" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I11" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J11" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K11" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H12" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I12" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J12" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K12" s="3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1055,6 +790,332 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA526FA-D473-0C43-85F7-C0A500F4351B}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2040</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H2" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I2" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J2" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K2" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H3" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I3" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J3" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K3" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H4" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I4" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J4" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K4" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K5" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I6" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K6" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H7" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I7" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J7" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K7" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H8" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I8" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J8" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K8" s="3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S141"/>
   <sheetViews>
@@ -1062,19 +1123,19 @@
       <selection activeCell="Q129" sqref="Q129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1115,7 +1176,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>17</v>
       </c>
@@ -1156,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>17</v>
       </c>
@@ -1197,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>17</v>
       </c>
@@ -1238,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>17</v>
       </c>
@@ -1279,7 +1340,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>17</v>
       </c>
@@ -1320,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>17</v>
       </c>
@@ -1361,7 +1422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>17</v>
       </c>
@@ -1402,7 +1463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>18</v>
       </c>
@@ -1443,7 +1504,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>18</v>
       </c>
@@ -1484,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>18</v>
       </c>
@@ -1525,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>18</v>
       </c>
@@ -1566,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>18</v>
       </c>
@@ -1607,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>18</v>
       </c>
@@ -1648,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>18</v>
       </c>
@@ -1689,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1730,7 +1791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1771,7 +1832,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -1812,7 +1873,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -1853,7 +1914,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>14</v>
       </c>
@@ -1894,7 +1955,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>14</v>
       </c>
@@ -1935,7 +1996,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -1976,7 +2037,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>15</v>
       </c>
@@ -2017,7 +2078,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>15</v>
       </c>
@@ -2058,7 +2119,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>15</v>
       </c>
@@ -2099,7 +2160,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>15</v>
       </c>
@@ -2140,7 +2201,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>15</v>
       </c>
@@ -2181,7 +2242,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>15</v>
       </c>
@@ -2222,7 +2283,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>15</v>
       </c>
@@ -2263,7 +2324,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>17</v>
       </c>
@@ -2304,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>17</v>
       </c>
@@ -2345,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -2386,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>17</v>
       </c>
@@ -2427,7 +2488,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>17</v>
       </c>
@@ -2468,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>17</v>
       </c>
@@ -2509,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>17</v>
       </c>
@@ -2550,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>18</v>
       </c>
@@ -2591,7 +2652,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>18</v>
       </c>
@@ -2632,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>18</v>
       </c>
@@ -2673,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>18</v>
       </c>
@@ -2714,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>18</v>
       </c>
@@ -2755,7 +2816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>18</v>
       </c>
@@ -2796,7 +2857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>18</v>
       </c>
@@ -2837,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>14</v>
       </c>
@@ -2878,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>14</v>
       </c>
@@ -2919,7 +2980,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>14</v>
       </c>
@@ -2960,7 +3021,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>14</v>
       </c>
@@ -3001,7 +3062,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>14</v>
       </c>
@@ -3042,7 +3103,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>14</v>
       </c>
@@ -3083,7 +3144,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>14</v>
       </c>
@@ -3124,7 +3185,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>15</v>
       </c>
@@ -3165,7 +3226,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>15</v>
       </c>
@@ -3206,7 +3267,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>15</v>
       </c>
@@ -3247,7 +3308,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>15</v>
       </c>
@@ -3288,7 +3349,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>15</v>
       </c>
@@ -3329,7 +3390,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>15</v>
       </c>
@@ -3370,7 +3431,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>15</v>
       </c>
@@ -3411,7 +3472,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>17</v>
       </c>
@@ -3452,7 +3513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>17</v>
       </c>
@@ -3493,7 +3554,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>17</v>
       </c>
@@ -3534,7 +3595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>17</v>
       </c>
@@ -3575,7 +3636,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>17</v>
       </c>
@@ -3616,7 +3677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>17</v>
       </c>
@@ -3657,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>17</v>
       </c>
@@ -3698,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>18</v>
       </c>
@@ -3739,7 +3800,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>18</v>
       </c>
@@ -3780,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>18</v>
       </c>
@@ -3821,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>18</v>
       </c>
@@ -3862,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>18</v>
       </c>
@@ -3903,7 +3964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>18</v>
       </c>
@@ -3944,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>18</v>
       </c>
@@ -3985,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>14</v>
       </c>
@@ -4026,7 +4087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>14</v>
       </c>
@@ -4067,7 +4128,7 @@
         <v>0.90249999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>14</v>
       </c>
@@ -4108,7 +4169,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>14</v>
       </c>
@@ -4149,7 +4210,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>14</v>
       </c>
@@ -4190,7 +4251,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>14</v>
       </c>
@@ -4231,7 +4292,7 @@
         <v>0.94524999999999992</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>14</v>
       </c>
@@ -4272,7 +4333,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>15</v>
       </c>
@@ -4313,7 +4374,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>15</v>
       </c>
@@ -4354,7 +4415,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>15</v>
       </c>
@@ -4395,7 +4456,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>15</v>
       </c>
@@ -4436,7 +4497,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>15</v>
       </c>
@@ -4477,7 +4538,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>15</v>
       </c>
@@ -4518,7 +4579,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>15</v>
       </c>
@@ -4559,7 +4620,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>17</v>
       </c>
@@ -4600,7 +4661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>17</v>
       </c>
@@ -4641,7 +4702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>17</v>
       </c>
@@ -4682,7 +4743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>17</v>
       </c>
@@ -4723,7 +4784,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>17</v>
       </c>
@@ -4764,7 +4825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>17</v>
       </c>
@@ -4805,7 +4866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>17</v>
       </c>
@@ -4846,7 +4907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>18</v>
       </c>
@@ -4887,7 +4948,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>18</v>
       </c>
@@ -4928,7 +4989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>18</v>
       </c>
@@ -4969,7 +5030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>18</v>
       </c>
@@ -5010,7 +5071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>18</v>
       </c>
@@ -5051,7 +5112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>18</v>
       </c>
@@ -5092,7 +5153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>18</v>
       </c>
@@ -5133,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>14</v>
       </c>
@@ -5174,7 +5235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>14</v>
       </c>
@@ -5215,7 +5276,7 @@
         <v>0.90249999999999997</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>14</v>
       </c>
@@ -5256,7 +5317,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>14</v>
       </c>
@@ -5297,7 +5358,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>14</v>
       </c>
@@ -5338,7 +5399,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>14</v>
       </c>
@@ -5379,7 +5440,7 @@
         <v>0.94524999999999992</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>14</v>
       </c>
@@ -5420,7 +5481,7 @@
         <v>0.95474999999999988</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>15</v>
       </c>
@@ -5461,7 +5522,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>15</v>
       </c>
@@ -5502,7 +5563,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>15</v>
       </c>
@@ -5543,7 +5604,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>15</v>
       </c>
@@ -5584,7 +5645,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>15</v>
       </c>
@@ -5625,7 +5686,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>15</v>
       </c>
@@ -5666,7 +5727,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>15</v>
       </c>
@@ -5707,7 +5768,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>17</v>
       </c>
@@ -5748,7 +5809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>17</v>
       </c>
@@ -5789,7 +5850,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>17</v>
       </c>
@@ -5830,7 +5891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>17</v>
       </c>
@@ -5871,7 +5932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>17</v>
       </c>
@@ -5912,7 +5973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>17</v>
       </c>
@@ -5953,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>17</v>
       </c>
@@ -5994,7 +6055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>18</v>
       </c>
@@ -6035,7 +6096,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>18</v>
       </c>
@@ -6076,7 +6137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>18</v>
       </c>
@@ -6117,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>18</v>
       </c>
@@ -6158,7 +6219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>18</v>
       </c>
@@ -6199,7 +6260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>18</v>
       </c>
@@ -6240,7 +6301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>18</v>
       </c>
@@ -6281,7 +6342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>14</v>
       </c>
@@ -6322,7 +6383,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>14</v>
       </c>
@@ -6363,7 +6424,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>14</v>
       </c>
@@ -6409,7 +6470,7 @@
       <c r="R130" s="7"/>
       <c r="S130" s="7"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>14</v>
       </c>
@@ -6450,7 +6511,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>14</v>
       </c>
@@ -6491,7 +6552,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>14</v>
       </c>
@@ -6532,7 +6593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>14</v>
       </c>
@@ -6573,7 +6634,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>15</v>
       </c>
@@ -6614,7 +6675,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>15</v>
       </c>
@@ -6655,7 +6716,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>15</v>
       </c>
@@ -6696,7 +6757,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>15</v>
       </c>
@@ -6737,7 +6798,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>15</v>
       </c>
@@ -6778,7 +6839,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>15</v>
       </c>
@@ -6819,7 +6880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>15</v>
       </c>
@@ -6866,34 +6927,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="40.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
-    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="22.5" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" customWidth="1"/>
-    <col min="13" max="13" width="18.453125" customWidth="1"/>
-    <col min="14" max="14" width="16.36328125" customWidth="1"/>
-    <col min="15" max="15" width="17.81640625" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="18.5" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -6922,7 +6983,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>45</v>
       </c>
@@ -6956,7 +7017,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>43</v>
       </c>
@@ -6990,7 +7051,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>42</v>
       </c>
@@ -7024,7 +7085,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>32</v>
       </c>
@@ -7058,7 +7119,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>31</v>
       </c>
@@ -7092,7 +7153,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>29</v>
       </c>
@@ -7126,7 +7187,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>34</v>
       </c>
@@ -7165,7 +7226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -7173,13 +7234,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -7188,7 +7249,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>61</v>
       </c>
@@ -7197,7 +7258,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -7206,7 +7267,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>63</v>
       </c>

</xml_diff>